<commit_message>
added functions, typehints and docstrings to exercise 1 and 2
</commit_message>
<xml_diff>
--- a/reportRetail.xlsx
+++ b/reportRetail.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,595 +434,487 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Category</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Sales</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>contribution %</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>All other gen. merchandise stores</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>37476</v>
+      </c>
       <c r="C2" t="n">
-        <v>37476</v>
-      </c>
-      <c r="D2" t="n">
         <v>0.2204848654931125</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Automobile and other motor vehicle dealers</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>421247</v>
+      </c>
       <c r="C3" t="n">
-        <v>421247</v>
-      </c>
-      <c r="D3" t="n">
         <v>2.478348493285761</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Automotive parts, acc., and tire stores</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>37875</v>
+      </c>
       <c r="C4" t="n">
-        <v>37875</v>
-      </c>
-      <c r="D4" t="n">
         <v>0.2228323268372194</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Beer, wine and liquor stores</t>
         </is>
       </c>
+      <c r="B5" t="n">
+        <v>27921</v>
+      </c>
       <c r="C5" t="n">
-        <v>27921</v>
-      </c>
-      <c r="D5" t="n">
         <v>0.164269343831604</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Building mat. and garden equip. and supplies dealers</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>170352</v>
+      </c>
       <c r="C6" t="n">
-        <v>170352</v>
-      </c>
-      <c r="D6" t="n">
         <v>1.002242443336608</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Building mat. and supplies dealers</t>
         </is>
       </c>
+      <c r="B7" t="n">
+        <v>149024</v>
+      </c>
       <c r="C7" t="n">
-        <v>149024</v>
-      </c>
-      <c r="D7" t="n">
         <v>0.8767621036195324</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Clothing and clothing access. stores</t>
         </is>
       </c>
+      <c r="B8" t="n">
+        <v>67154</v>
+      </c>
       <c r="C8" t="n">
-        <v>67154</v>
-      </c>
-      <c r="D8" t="n">
         <v>0.3950912759452576</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Clothing stores</t>
         </is>
       </c>
+      <c r="B9" t="n">
+        <v>47047</v>
+      </c>
       <c r="C9" t="n">
-        <v>47047</v>
-      </c>
-      <c r="D9" t="n">
         <v>0.2767945209428558</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Department stores</t>
         </is>
       </c>
+      <c r="B10" t="n">
+        <v>45256</v>
+      </c>
       <c r="C10" t="n">
-        <v>45256</v>
-      </c>
-      <c r="D10" t="n">
         <v>0.2662574200223156</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Electronic shopping and mail order houses</t>
         </is>
       </c>
+      <c r="B11" t="n">
+        <v>340496</v>
+      </c>
       <c r="C11" t="n">
-        <v>340496</v>
-      </c>
-      <c r="D11" t="n">
         <v>2.003261147426162</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Electronics and appliance stores</t>
         </is>
       </c>
+      <c r="B12" t="n">
+        <v>31760</v>
+      </c>
       <c r="C12" t="n">
-        <v>31760</v>
-      </c>
-      <c r="D12" t="n">
         <v>0.186855569646207</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Food and beverage stores</t>
         </is>
       </c>
+      <c r="B13" t="n">
+        <v>354169</v>
+      </c>
       <c r="C13" t="n">
-        <v>354169</v>
-      </c>
-      <c r="D13" t="n">
         <v>2.083704352834618</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Food services and drinking places</t>
         </is>
       </c>
+      <c r="B14" t="n">
+        <v>246070</v>
+      </c>
       <c r="C14" t="n">
-        <v>246070</v>
-      </c>
-      <c r="D14" t="n">
         <v>1.447718829434576</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Fuel dealers</t>
         </is>
       </c>
+      <c r="B15" t="n">
+        <v>10134</v>
+      </c>
       <c r="C15" t="n">
-        <v>10134</v>
-      </c>
-      <c r="D15" t="n">
         <v>0.05962198812325761</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Furniture and home furnishings stores</t>
         </is>
       </c>
+      <c r="B16" t="n">
+        <v>39464</v>
+      </c>
       <c r="C16" t="n">
-        <v>39464</v>
-      </c>
-      <c r="D16" t="n">
         <v>0.2321809886812945</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Furniture, home furn, electronics, and appliance stores</t>
         </is>
       </c>
+      <c r="B17" t="n">
+        <v>71224</v>
+      </c>
       <c r="C17" t="n">
-        <v>71224</v>
-      </c>
-      <c r="D17" t="n">
         <v>0.4190365583275015</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Gasoline stations</t>
         </is>
       </c>
+      <c r="B18" t="n">
+        <v>173570</v>
+      </c>
       <c r="C18" t="n">
-        <v>173570</v>
-      </c>
-      <c r="D18" t="n">
         <v>1.021175101495345</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>General merchandise stores</t>
         </is>
       </c>
+      <c r="B19" t="n">
+        <v>300482</v>
+      </c>
       <c r="C19" t="n">
-        <v>300482</v>
-      </c>
-      <c r="D19" t="n">
         <v>1.767844309774294</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Grocery stores</t>
         </is>
       </c>
+      <c r="B20" t="n">
+        <v>317133</v>
+      </c>
       <c r="C20" t="n">
-        <v>317133</v>
-      </c>
-      <c r="D20" t="n">
         <v>1.865808166517965</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
+      <c r="A21" t="inlineStr">
         <is>
           <t>Health and personal care stores</t>
         </is>
       </c>
+      <c r="B21" t="n">
+        <v>145813</v>
+      </c>
       <c r="C21" t="n">
-        <v>145813</v>
-      </c>
-      <c r="D21" t="n">
         <v>0.857870628993148</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
+      <c r="A22" t="inlineStr">
         <is>
           <t>Men's clothing stores</t>
         </is>
       </c>
+      <c r="B22" t="n">
+        <v>1789</v>
+      </c>
       <c r="C22" t="n">
-        <v>1789</v>
-      </c>
-      <c r="D22" t="n">
         <v>0.01052533419701084</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>Miscellaneous stores retailers</t>
         </is>
       </c>
+      <c r="B23" t="n">
+        <v>50505</v>
+      </c>
       <c r="C23" t="n">
-        <v>50505</v>
-      </c>
-      <c r="D23" t="n">
         <v>0.297139185925116</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>Motor vehicle and parts dealers</t>
         </is>
       </c>
+      <c r="B24" t="n">
+        <v>459122</v>
+      </c>
       <c r="C24" t="n">
-        <v>459122</v>
-      </c>
-      <c r="D24" t="n">
         <v>2.70118082012298</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
+      <c r="A25" t="inlineStr">
         <is>
           <t>Nonstore retailers</t>
         </is>
       </c>
+      <c r="B25" t="n">
+        <v>373480</v>
+      </c>
       <c r="C25" t="n">
-        <v>373480</v>
-      </c>
-      <c r="D25" t="n">
         <v>2.197317951872336</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
+      <c r="A26" t="inlineStr">
         <is>
           <t>Other general merchandise stores</t>
         </is>
       </c>
+      <c r="B26" t="n">
+        <v>255226</v>
+      </c>
       <c r="C26" t="n">
-        <v>255226</v>
-      </c>
-      <c r="D26" t="n">
         <v>1.501586889751978</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Pharmacies and drug stores</t>
         </is>
       </c>
+      <c r="B27" t="n">
+        <v>126520</v>
+      </c>
       <c r="C27" t="n">
-        <v>126520</v>
-      </c>
-      <c r="D27" t="n">
         <v>0.7443629304671948</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
+      <c r="A28" t="inlineStr">
         <is>
           <t>Retail and food services sales, total</t>
         </is>
       </c>
+      <c r="B28" t="n">
+        <v>2441122</v>
+      </c>
       <c r="C28" t="n">
-        <v>2441122</v>
-      </c>
-      <c r="D28" t="n">
         <v>14.36200383771688</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
+      <c r="A29" t="inlineStr">
         <is>
           <t>Retail sales and food services excl gasoline stations</t>
         </is>
       </c>
+      <c r="B29" t="n">
+        <v>2267552</v>
+      </c>
       <c r="C29" t="n">
-        <v>2267552</v>
-      </c>
-      <c r="D29" t="n">
         <v>13.34082873622154</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
+      <c r="A30" t="inlineStr">
         <is>
           <t>Retail sales and food services excl motor vehicle and parts</t>
         </is>
       </c>
+      <c r="B30" t="n">
+        <v>1982000</v>
+      </c>
       <c r="C30" t="n">
-        <v>1982000</v>
-      </c>
-      <c r="D30" t="n">
         <v>11.6608230175939</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
+      <c r="A31" t="inlineStr">
         <is>
           <t>Retail sales and food services excl motor vehicle and parts and gasoline stations</t>
         </is>
       </c>
+      <c r="B31" t="n">
+        <v>1808430</v>
+      </c>
       <c r="C31" t="n">
-        <v>1808430</v>
-      </c>
-      <c r="D31" t="n">
         <v>10.63964791609856</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
+      <c r="A32" t="inlineStr">
         <is>
           <t>Retail sales, total</t>
         </is>
       </c>
+      <c r="B32" t="n">
+        <v>2195052</v>
+      </c>
       <c r="C32" t="n">
-        <v>2195052</v>
-      </c>
-      <c r="D32" t="n">
         <v>12.9142850082823</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
+      <c r="A33" t="inlineStr">
         <is>
           <t>Retail sales, total (excl. motor vehicle and parts dealers)</t>
         </is>
       </c>
+      <c r="B33" t="n">
+        <v>1735930</v>
+      </c>
       <c r="C33" t="n">
-        <v>1735930</v>
-      </c>
-      <c r="D33" t="n">
         <v>10.21310418815932</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Shoe stores</t>
         </is>
       </c>
+      <c r="B34" t="n">
+        <v>9879</v>
+      </c>
       <c r="C34" t="n">
-        <v>9879</v>
-      </c>
-      <c r="D34" t="n">
         <v>0.05812173087326444</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
+      <c r="A35" t="inlineStr">
         <is>
           <t>Sporting goods, hobby, musical instrument, and book stores</t>
         </is>
       </c>
+      <c r="B35" t="n">
+        <v>29181</v>
+      </c>
       <c r="C35" t="n">
-        <v>29181</v>
-      </c>
-      <c r="D35" t="n">
         <v>0.1716823796550997</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
+      <c r="A36" t="inlineStr">
         <is>
           <t>Warehouse clubs and superstores</t>
         </is>
       </c>
+      <c r="B36" t="n">
+        <v>217750</v>
+      </c>
       <c r="C36" t="n">
-        <v>217750</v>
-      </c>
-      <c r="D36" t="n">
         <v>1.281102024258866</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
+      <c r="A37" t="inlineStr">
         <is>
           <t>Women's clothing stores</t>
         </is>
       </c>
+      <c r="B37" t="n">
+        <v>9880</v>
+      </c>
       <c r="C37" t="n">
-        <v>9880</v>
-      </c>
-      <c r="D37" t="n">
         <v>0.05812761423502912</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added describing names to data results, concatenated and exported all results into reportRetail
</commit_message>
<xml_diff>
--- a/reportRetail.xlsx
+++ b/reportRetail.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,16 @@
           <t>contribution %</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Month</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Sales Manager</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -462,6 +472,8 @@
       <c r="C2" t="n">
         <v>0.2204848654931125</v>
       </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -475,6 +487,8 @@
       <c r="C3" t="n">
         <v>2.478348493285761</v>
       </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -488,6 +502,8 @@
       <c r="C4" t="n">
         <v>0.2228323268372194</v>
       </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -501,6 +517,8 @@
       <c r="C5" t="n">
         <v>0.164269343831604</v>
       </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -514,6 +532,8 @@
       <c r="C6" t="n">
         <v>1.002242443336608</v>
       </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -527,6 +547,8 @@
       <c r="C7" t="n">
         <v>0.8767621036195324</v>
       </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -540,6 +562,8 @@
       <c r="C8" t="n">
         <v>0.3950912759452576</v>
       </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -553,6 +577,8 @@
       <c r="C9" t="n">
         <v>0.2767945209428558</v>
       </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -566,6 +592,8 @@
       <c r="C10" t="n">
         <v>0.2662574200223156</v>
       </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -579,6 +607,8 @@
       <c r="C11" t="n">
         <v>2.003261147426162</v>
       </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -592,6 +622,8 @@
       <c r="C12" t="n">
         <v>0.186855569646207</v>
       </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -605,6 +637,8 @@
       <c r="C13" t="n">
         <v>2.083704352834618</v>
       </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -618,6 +652,8 @@
       <c r="C14" t="n">
         <v>1.447718829434576</v>
       </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -631,6 +667,8 @@
       <c r="C15" t="n">
         <v>0.05962198812325761</v>
       </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -644,6 +682,8 @@
       <c r="C16" t="n">
         <v>0.2321809886812945</v>
       </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -657,6 +697,8 @@
       <c r="C17" t="n">
         <v>0.4190365583275015</v>
       </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -670,6 +712,8 @@
       <c r="C18" t="n">
         <v>1.021175101495345</v>
       </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -683,6 +727,8 @@
       <c r="C19" t="n">
         <v>1.767844309774294</v>
       </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -696,6 +742,8 @@
       <c r="C20" t="n">
         <v>1.865808166517965</v>
       </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -709,6 +757,8 @@
       <c r="C21" t="n">
         <v>0.857870628993148</v>
       </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -722,6 +772,8 @@
       <c r="C22" t="n">
         <v>0.01052533419701084</v>
       </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -735,6 +787,8 @@
       <c r="C23" t="n">
         <v>0.297139185925116</v>
       </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -748,6 +802,8 @@
       <c r="C24" t="n">
         <v>2.70118082012298</v>
       </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -761,6 +817,8 @@
       <c r="C25" t="n">
         <v>2.197317951872336</v>
       </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -774,6 +832,8 @@
       <c r="C26" t="n">
         <v>1.501586889751978</v>
       </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -787,6 +847,8 @@
       <c r="C27" t="n">
         <v>0.7443629304671948</v>
       </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -800,6 +862,8 @@
       <c r="C28" t="n">
         <v>14.36200383771688</v>
       </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -813,6 +877,8 @@
       <c r="C29" t="n">
         <v>13.34082873622154</v>
       </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -826,6 +892,8 @@
       <c r="C30" t="n">
         <v>11.6608230175939</v>
       </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -839,6 +907,8 @@
       <c r="C31" t="n">
         <v>10.63964791609856</v>
       </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -852,6 +922,8 @@
       <c r="C32" t="n">
         <v>12.9142850082823</v>
       </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -865,6 +937,8 @@
       <c r="C33" t="n">
         <v>10.21310418815932</v>
       </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -878,6 +952,8 @@
       <c r="C34" t="n">
         <v>0.05812173087326444</v>
       </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -891,6 +967,8 @@
       <c r="C35" t="n">
         <v>0.1716823796550997</v>
       </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -904,6 +982,8 @@
       <c r="C36" t="n">
         <v>1.281102024258866</v>
       </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -916,6 +996,203 @@
       </c>
       <c r="C37" t="n">
         <v>0.05812761423502912</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="n">
+        <v>2954149</v>
+      </c>
+      <c r="C38" t="n">
+        <v>17.38032727376488</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="n">
+        <v>3597561</v>
+      </c>
+      <c r="C39" t="n">
+        <v>21.16575283350057</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Feburary</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="n">
+        <v>3610492</v>
+      </c>
+      <c r="C40" t="n">
+        <v>21.24183058447963</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>January</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="n">
+        <v>3422543</v>
+      </c>
+      <c r="C41" t="n">
+        <v>20.13605862416997</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="n">
+        <v>3412340</v>
+      </c>
+      <c r="C42" t="n">
+        <v>20.07603068408495</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="n">
+        <v>29181</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.1716823796550997</v>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Chen Cho</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="n">
+        <v>6750743</v>
+      </c>
+      <c r="C44" t="n">
+        <v>39.71706324937482</v>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Dominique Kai</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="n">
+        <v>2544106</v>
+      </c>
+      <c r="C45" t="n">
+        <v>14.96789596569059</v>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Donald Ducker</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="n">
+        <v>2540790</v>
+      </c>
+      <c r="C46" t="n">
+        <v>14.94838673807891</v>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Jane Maria</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="n">
+        <v>1297791</v>
+      </c>
+      <c r="C47" t="n">
+        <v>7.635373947944603</v>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="n">
+        <v>355958</v>
+      </c>
+      <c r="C48" t="n">
+        <v>2.094229687031629</v>
+      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Marc Jensen</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="n">
+        <v>515025</v>
+      </c>
+      <c r="C49" t="n">
+        <v>3.030078392853834</v>
+      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Martin Miller</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="n">
+        <v>2963491</v>
+      </c>
+      <c r="C50" t="n">
+        <v>17.43528963937052</v>
+      </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Vicky Dullo</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>